<commit_message>
Hazle pull a este
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -29,19 +29,19 @@
     <t>torta</t>
   </si>
   <si>
-    <t>1.0-huevos,2.0-harinita,1.0-vainilla,5.0-leche,</t>
+    <t>5.0-leche,1.0-vainilla,1.0-huevos,2.0-harinita,</t>
   </si>
   <si>
     <t>kuchen manzana</t>
   </si>
   <si>
-    <t>5.0-huevos,1.0-harinita,2.0-manzana,</t>
+    <t>2.0-manzana,5.0-huevos,1.0-harinita,</t>
   </si>
   <si>
     <t>queque</t>
   </si>
   <si>
-    <t>2.0-huevos,5.0-harinita,1.0-vainilla,</t>
+    <t>1.0-vainilla,2.0-huevos,5.0-harinita,</t>
   </si>
   <si>
     <t>tartaleta durazno</t>
@@ -53,7 +53,7 @@
     <t>pie de limon</t>
   </si>
   <si>
-    <t>5.0-huevos,4.0-harinita,1.0-crema,5.0-merengue,2.0-limon,</t>
+    <t>5.0-merengue,2.0-limon,1.0-crema,5.0-huevos,4.0-harinita,</t>
   </si>
   <si>
     <t>testito</t>

</xml_diff>

<commit_message>
metodo dias restantes para el retiro, al cancelar pedido no se borra,validar tiempo elaboracion
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -53,13 +53,19 @@
     <t>pie de limon</t>
   </si>
   <si>
-    <t>5.0-merengue,2.0-limon,1.0-crema,5.0-huevos,4.0-harinita,</t>
+    <t>5.0-merengue,2.0-limon,5.0-huevos,4.0-harinita,1.0-crema,</t>
   </si>
   <si>
     <t>testito</t>
   </si>
   <si>
     <t>1.0-harinita,</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>2.0-harinita,</t>
   </si>
 </sst>
 </file>
@@ -208,6 +214,20 @@
         <v>12.0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-3.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Merge Manual con cosas anteriores
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -29,31 +29,31 @@
     <t>torta</t>
   </si>
   <si>
-    <t>5.0-leche,1.0-vainilla,1.0-huevos,2.0-harinita,</t>
+    <t>2.0-harinita,1.0-huevos,1.0-vainilla,5.0-leche,</t>
   </si>
   <si>
     <t>kuchen manzana</t>
   </si>
   <si>
-    <t>2.0-manzana,5.0-huevos,1.0-harinita,</t>
+    <t>1.0-harinita,5.0-huevos,2.0-manzana,</t>
   </si>
   <si>
     <t>queque</t>
   </si>
   <si>
-    <t>1.0-vainilla,2.0-huevos,5.0-harinita,</t>
+    <t>5.0-harinita,2.0-huevos,1.0-vainilla,</t>
   </si>
   <si>
     <t>tartaleta durazno</t>
   </si>
   <si>
-    <t>5.0-huevos,5.0-harinita,</t>
+    <t>5.0-harinita,5.0-huevos,</t>
   </si>
   <si>
     <t>pie de limon</t>
   </si>
   <si>
-    <t>5.0-merengue,2.0-limon,1.0-crema,5.0-huevos,4.0-harinita,</t>
+    <t>4.0-harinita,5.0-merengue,5.0-huevos,2.0-limon,1.0-crema,</t>
   </si>
   <si>
     <t>testito</t>

</xml_diff>

<commit_message>
validar tiempo de elaboracion
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -29,31 +29,31 @@
     <t>torta</t>
   </si>
   <si>
-    <t>5.0-leche,1.0-vainilla,1.0-huevos,2.0-harinita,</t>
+    <t>5.0-leche,1.0-vainilla,2.0-harinita,1.0-huevos,</t>
   </si>
   <si>
     <t>kuchen manzana</t>
   </si>
   <si>
-    <t>5.0-huevos,2.0-manzana,1.0-harinita,</t>
+    <t>2.0-manzana,1.0-harinita,5.0-huevos,</t>
   </si>
   <si>
     <t>queque</t>
   </si>
   <si>
-    <t>1.0-vainilla,2.0-huevos,5.0-harinita,</t>
+    <t>1.0-vainilla,5.0-harinita,2.0-huevos,</t>
   </si>
   <si>
     <t>tartaleta durazno</t>
   </si>
   <si>
-    <t>5.0-huevos,5.0-harinita,</t>
+    <t>5.0-harinita,5.0-huevos,</t>
   </si>
   <si>
     <t>pie de limon</t>
   </si>
   <si>
-    <t>5.0-merengue,2.0-limon,1.0-crema,5.0-huevos,4.0-harinita,</t>
+    <t>1.0-crema,2.0-limon,4.0-harinita,5.0-huevos,5.0-merengue,</t>
   </si>
   <si>
     <t>testito</t>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>2.0-harinita,</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -228,6 +231,20 @@
         <v>-3.0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix No inicia, sólo envía correo
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>1.0-Huevos (unidad),1.0-Vainilla (ml),2.0-Harina  (kg),3.0-Leche (litros),</t>
+    <t>1.0-Huevos (unidad),3.0-Leche (litros),1.0-Vainilla (ml),2.0-Harina  (kg),</t>
   </si>
   <si>
     <t>0</t>
@@ -65,7 +65,7 @@
     <t>Cupcake</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),0.1-Vainilla (ml),0.3-Harina  (kg),0.2-Leche (litros),</t>
+    <t>2.0-Huevos (unidad),0.2-Leche (litros),0.1-Vainilla (ml),0.3-Harina  (kg),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Stash antes del merge
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>1.0-Huevos (unidad),3.0-Leche (litros),1.0-Vainilla (ml),2.0-Harina  (kg),</t>
+    <t>3.0-Leche (litros),2.0-Harina  (kg),1.0-Vainilla (ml),1.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>0</t>
@@ -41,31 +41,31 @@
     <t>Kuchen Manzana</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),2.0-Harina  (kg),</t>
+    <t>2.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Queque</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),1.0-Vainilla (ml),5.0-Harina  (kg),</t>
+    <t>5.0-Harina  (kg),1.0-Vainilla (ml),2.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),5.0-Harina  (kg),</t>
+    <t>5.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),2.0-Limon (unidad),5.0-Crema (litros),4.0-Harina  (kg),</t>
+    <t>2.0-Limon (unidad),4.0-Harina  (kg),5.0-Huevos (unidad),5.0-Crema (litros),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),0.2-Leche (litros),0.1-Vainilla (ml),0.3-Harina  (kg),</t>
+    <t>0.2-Leche (litros),0.3-Harina  (kg),0.1-Vainilla (ml),2.0-Huevos (unidad),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Comentarios de clases y patron proxy
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,10 +32,10 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>1.0-Huevos (unidad),3.0-Leche (litros),1.0-Vainilla (ml),2.0-Harina  (kg),</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>1.0-Huevos (unidad),3.0-Leche (litros),2.0-Harina  (kg),1.0-Vainilla (ml),</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>Kuchen Manzana</t>
@@ -47,7 +47,7 @@
     <t>Queque</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),1.0-Vainilla (ml),5.0-Harina  (kg),</t>
+    <t>2.0-Huevos (unidad),5.0-Harina  (kg),1.0-Vainilla (ml),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
@@ -59,13 +59,13 @@
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),2.0-Limon (unidad),5.0-Crema (litros),4.0-Harina  (kg),</t>
+    <t>5.0-Huevos (unidad),5.0-Crema (litros),4.0-Harina  (kg),2.0-Limon (unidad),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),0.2-Leche (litros),0.1-Vainilla (ml),0.3-Harina  (kg),</t>
+    <t>2.0-Huevos (unidad),0.2-Leche (litros),0.3-Harina  (kg),0.1-Vainilla (ml),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Revisión y modificación nombres de atributos, objetos, etc
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>2.0-Harina  (kg),1.0-Huevos (unidad),1.0-Vainilla (ml),3.0-Leche (litros),</t>
+    <t>1.0-Huevos (unidad),3.0-Leche (litros),1.0-Vainilla (ml),2.0-Harina  (kg),</t>
   </si>
   <si>
     <t>0</t>
@@ -41,31 +41,31 @@
     <t>Kuchen Manzana</t>
   </si>
   <si>
-    <t>2.0-Harina  (kg),5.0-Huevos (unidad),</t>
+    <t>5.0-Huevos (unidad),2.0-Harina  (kg),</t>
   </si>
   <si>
     <t>Queque</t>
   </si>
   <si>
-    <t>5.0-Harina  (kg),2.0-Huevos (unidad),1.0-Vainilla (ml),</t>
+    <t>2.0-Huevos (unidad),1.0-Vainilla (ml),5.0-Harina  (kg),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
   </si>
   <si>
-    <t>5.0-Harina  (kg),5.0-Huevos (unidad),</t>
+    <t>5.0-Huevos (unidad),5.0-Harina  (kg),</t>
   </si>
   <si>
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>4.0-Harina  (kg),2.0-Limon (unidad),5.0-Huevos (unidad),5.0-Crema (litros),</t>
+    <t>5.0-Huevos (unidad),2.0-Limon (unidad),4.0-Harina  (kg),5.0-Crema (litros),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>0.3-Harina  (kg),2.0-Huevos (unidad),0.1-Vainilla (ml),0.2-Leche (litros),</t>
+    <t>2.0-Huevos (unidad),0.2-Leche (litros),0.1-Vainilla (ml),0.3-Harina  (kg),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Genera arrayList de los productos más vendidos
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>1.0-Huevos (unidad),3.0-Leche (litros),1.0-Vainilla (ml),2.0-Harina  (kg),</t>
+    <t>3.0-Leche (litros),2.0-Harina  (kg),1.0-Vainilla (ml),1.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>0</t>
@@ -41,31 +41,31 @@
     <t>Kuchen Manzana</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),2.0-Harina  (kg),</t>
+    <t>2.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Queque</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),1.0-Vainilla (ml),5.0-Harina  (kg),</t>
+    <t>5.0-Harina  (kg),1.0-Vainilla (ml),2.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),5.0-Harina  (kg),</t>
+    <t>5.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),2.0-Limon (unidad),4.0-Harina  (kg),5.0-Crema (litros),</t>
+    <t>5.0-Crema (litros),4.0-Harina  (kg),5.0-Huevos (unidad),2.0-Limon (unidad),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>2.0-Huevos (unidad),0.2-Leche (litros),0.1-Vainilla (ml),0.3-Harina  (kg),</t>
+    <t>0.2-Leche (litros),0.3-Harina  (kg),0.1-Vainilla (ml),2.0-Huevos (unidad),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Comentarios de clases y metodos package interfaz
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>1.0-Vainilla (ml),1.0-Huevos (unidad),3.0-Leche (litros),2.0-Harina  (kg),</t>
+    <t>2.0-Harina  (kg),1.0-Huevos (unidad),1.0-Vainilla (ml),3.0-Leche (litros),</t>
   </si>
   <si>
     <t>1</t>
@@ -41,31 +41,31 @@
     <t>Kuchen Manzana</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),2.0-Harina  (kg),</t>
+    <t>2.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Queque</t>
   </si>
   <si>
-    <t>1.0-Vainilla (ml),2.0-Huevos (unidad),5.0-Harina  (kg),</t>
+    <t>5.0-Harina  (kg),2.0-Huevos (unidad),1.0-Vainilla (ml),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
   </si>
   <si>
-    <t>5.0-Huevos (unidad),5.0-Harina  (kg),</t>
+    <t>5.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>2.0-Limon (unidad),5.0-Huevos (unidad),5.0-Crema (litros),4.0-Harina  (kg),</t>
+    <t>2.0-Limon (unidad),5.0-Crema (litros),4.0-Harina  (kg),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>0.1-Vainilla (ml),2.0-Huevos (unidad),0.2-Leche (litros),0.3-Harina  (kg),</t>
+    <t>0.3-Harina  (kg),2.0-Huevos (unidad),0.1-Vainilla (ml),0.2-Leche (litros),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Ahora no se puede interactuar directamente con el gráfico
Se evitó que se pudiese interactuar con el gráfico
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>1.0-Vainilla (ml),2.0-Harina  (kg),1.0-Huevos (unidad),3.0-Leche (litros),</t>
+    <t>3.0-Leche (litros),2.0-Harina  (kg),1.0-Vainilla (ml),1.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>1</t>
@@ -47,7 +47,7 @@
     <t>Queque</t>
   </si>
   <si>
-    <t>1.0-Vainilla (ml),5.0-Harina  (kg),2.0-Huevos (unidad),</t>
+    <t>5.0-Harina  (kg),1.0-Vainilla (ml),2.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
@@ -59,13 +59,13 @@
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>2.0-Limon (unidad),5.0-Crema (litros),4.0-Harina  (kg),5.0-Huevos (unidad),</t>
+    <t>2.0-Limon (unidad),4.0-Harina  (kg),5.0-Crema (litros),5.0-Huevos (unidad),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>0.1-Vainilla (ml),0.3-Harina  (kg),2.0-Huevos (unidad),0.2-Leche (litros),</t>
+    <t>0.2-Leche (litros),0.3-Harina  (kg),0.1-Vainilla (ml),2.0-Huevos (unidad),</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Correccion de errores reportados
</commit_message>
<xml_diff>
--- a/Nana&Rene/Productos.xlsx
+++ b/Nana&Rene/Productos.xlsx
@@ -32,7 +32,7 @@
     <t>Torta</t>
   </si>
   <si>
-    <t>3.0-Leche (litros),2.0-Harina  (kg),1.0-Vainilla (ml),1.0-Huevos (unidad),</t>
+    <t>3.0-Leche (litros),1.0-Huevos (unidad),2.0-Harina  (kg),1.0-Vainilla (ml),</t>
   </si>
   <si>
     <t>1</t>
@@ -41,31 +41,31 @@
     <t>Kuchen Manzana</t>
   </si>
   <si>
-    <t>2.0-Harina  (kg),5.0-Huevos (unidad),</t>
+    <t>5.0-Huevos (unidad),2.0-Harina  (kg),</t>
   </si>
   <si>
     <t>Queque</t>
   </si>
   <si>
-    <t>5.0-Harina  (kg),1.0-Vainilla (ml),2.0-Huevos (unidad),</t>
+    <t>2.0-Huevos (unidad),5.0-Harina  (kg),1.0-Vainilla (ml),</t>
   </si>
   <si>
     <t>Tartaleta Durazno</t>
   </si>
   <si>
-    <t>5.0-Harina  (kg),5.0-Huevos (unidad),</t>
+    <t>5.0-Huevos (unidad),5.0-Harina  (kg),</t>
   </si>
   <si>
     <t>Pie de Limon</t>
   </si>
   <si>
-    <t>2.0-Limon (unidad),4.0-Harina  (kg),5.0-Crema (litros),5.0-Huevos (unidad),</t>
+    <t>2.0-Limon (unidad),5.0-Crema (litros),5.0-Huevos (unidad),4.0-Harina  (kg),</t>
   </si>
   <si>
     <t>Cupcake</t>
   </si>
   <si>
-    <t>0.2-Leche (litros),0.3-Harina  (kg),0.1-Vainilla (ml),2.0-Huevos (unidad),</t>
+    <t>0.2-Leche (litros),2.0-Huevos (unidad),0.3-Harina  (kg),0.1-Vainilla (ml),</t>
   </si>
 </sst>
 </file>

</xml_diff>